<commit_message>
Actualización de la aplicación
</commit_message>
<xml_diff>
--- a/Proyecto/model/reports/PlantillaOrden.xlsx
+++ b/Proyecto/model/reports/PlantillaOrden.xlsx
@@ -479,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,15 +586,6 @@
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>